<commit_message>
2025.01.16 LeetCode 每日一题 Hot100
</commit_message>
<xml_diff>
--- a/LeetCode刷题记录.xlsx
+++ b/LeetCode刷题记录.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\develop\GithubRepo\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E01777F-AB4B-4630-93B8-24393E93641D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68EA486E-5567-432B-BB7E-BA5A35D103AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-163" yWindow="17" windowWidth="22106" windowHeight="11812" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11829" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="925" uniqueCount="509">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="953" uniqueCount="522">
   <si>
     <t>题目</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1344,10 +1344,6 @@
   </si>
   <si>
     <t>2024.11.11</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2024.11.25</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1880,6 +1876,58 @@
   </si>
   <si>
     <t>字符串、不使用Java内置方法实现</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3066. 超过阈值的最少操作数 II</t>
+  </si>
+  <si>
+    <t>2025.01.15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>最小堆（升序优先队列）、模拟</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>升序单调队列ArrayDeque存放下标，淘汰一定不是候选的，去掉窗口之外的</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>55. 右旋字符串（第八期模拟笔试）</t>
+  </si>
+  <si>
+    <t>int k =  Integer.parseInt(sc.nextLine());   // 标准写法</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>先整体再局部</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>28. 找出字符串中第一个匹配项的下标</t>
+  </si>
+  <si>
+    <t>459. 重复的子字符串</t>
+  </si>
+  <si>
+    <t>KMP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KMP的前缀表的值：以该位置结尾的字符串的最长相等前后缀的长度
+PR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2025.01.16</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3095. 或值至少 K 的最短子数组 I</t>
+  </si>
+  <si>
+    <t>return len==Integer.MAX_VALUE ? "" : s.substring(start, start+len); //[)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2342,10 +2390,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G191"/>
+  <dimension ref="A1:G196"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A158" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E173" sqref="E173"/>
+    <sheetView tabSelected="1" topLeftCell="A162" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G175" sqref="G175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -2388,13 +2436,13 @@
         <v>77</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="F2" s="6">
         <v>5</v>
@@ -2411,13 +2459,13 @@
         <v>41</v>
       </c>
       <c r="D3" s="8" t="s">
+        <v>377</v>
+      </c>
+      <c r="F3" s="6">
+        <v>3</v>
+      </c>
+      <c r="G3" s="14" t="s">
         <v>378</v>
-      </c>
-      <c r="F3" s="6">
-        <v>3</v>
-      </c>
-      <c r="G3" s="14" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2428,7 +2476,7 @@
         <v>13</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="F4" s="6">
         <v>3</v>
@@ -2445,13 +2493,13 @@
         <v>41</v>
       </c>
       <c r="D5" s="8" t="s">
+        <v>377</v>
+      </c>
+      <c r="F5" s="6">
+        <v>3</v>
+      </c>
+      <c r="G5" s="14" t="s">
         <v>378</v>
-      </c>
-      <c r="F5" s="6">
-        <v>3</v>
-      </c>
-      <c r="G5" s="14" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2485,7 +2533,7 @@
         <v>79</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="F7" s="6">
         <v>3</v>
@@ -2510,7 +2558,7 @@
         <v>13</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="F9" s="6">
         <v>3</v>
@@ -2527,7 +2575,7 @@
         <v>41</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E10" s="9" t="s">
         <v>92</v>
@@ -2547,7 +2595,7 @@
         <v>13</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="F11" s="6">
         <v>3</v>
@@ -2567,7 +2615,7 @@
         <v>94</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="E12" s="9" t="s">
         <v>14</v>
@@ -2647,7 +2695,7 @@
         <v>41</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="E16" s="9" t="s">
         <v>14</v>
@@ -2698,7 +2746,7 @@
         <v>13</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="F19" s="6">
         <v>3</v>
@@ -2721,7 +2769,7 @@
         <v>367</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="F20" s="6">
         <v>3</v>
@@ -2738,7 +2786,7 @@
         <v>94</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="E21" s="9" t="s">
         <v>124</v>
@@ -2747,7 +2795,7 @@
         <v>4</v>
       </c>
       <c r="G21" s="14" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2761,7 +2809,7 @@
         <v>27</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="F22" s="6">
         <v>3</v>
@@ -2769,30 +2817,30 @@
     </row>
     <row r="23" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="10" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D23" s="8" t="s">
+        <v>424</v>
+      </c>
+      <c r="G23" s="14" t="s">
         <v>425</v>
-      </c>
-      <c r="G23" s="14" t="s">
-        <v>426</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="10" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>41</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2806,7 +2854,7 @@
         <v>13</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="E25" s="9" t="s">
         <v>86</v>
@@ -2826,7 +2874,7 @@
         <v>13</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E26" s="9" t="s">
         <v>14</v>
@@ -2846,7 +2894,7 @@
         <v>41</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F27" s="6">
         <v>3</v>
@@ -2857,13 +2905,13 @@
         <v>191</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C28" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="E28" s="13" t="s">
         <v>332</v>
@@ -2872,7 +2920,7 @@
         <v>4</v>
       </c>
       <c r="G28" s="14" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2931,19 +2979,19 @@
         <v>197</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C32" s="7" t="s">
         <v>79</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="F32" s="6">
         <v>4</v>
       </c>
       <c r="G32" s="14" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2951,13 +2999,13 @@
         <v>93</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C33" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="E33" s="9" t="s">
         <v>14</v>
@@ -2966,7 +3014,7 @@
         <v>5</v>
       </c>
       <c r="G33" s="15" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -2974,19 +3022,19 @@
         <v>279</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C34" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="F34" s="6">
         <v>3</v>
       </c>
       <c r="G34" s="14" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3000,7 +3048,7 @@
         <v>13</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="F35" s="6">
         <v>3</v>
@@ -3020,7 +3068,7 @@
         <v>13</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="E36" s="9" t="s">
         <v>100</v>
@@ -3071,7 +3119,7 @@
         <v>6</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="E39" s="13" t="s">
         <v>328</v>
@@ -3105,7 +3153,7 @@
         <v>13</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="F41" s="6">
         <v>3</v>
@@ -3122,7 +3170,7 @@
         <v>79</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E42" s="9" t="s">
         <v>21</v>
@@ -3133,16 +3181,16 @@
     </row>
     <row r="43" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="10" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C43" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="F43" s="6">
         <v>1</v>
@@ -3156,7 +3204,7 @@
         <v>27</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="F44" s="6">
         <v>3</v>
@@ -3167,13 +3215,13 @@
         <v>194</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C45" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="F45" s="6">
         <v>5</v>
@@ -3193,13 +3241,13 @@
         <v>79</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="F46" s="6">
         <v>3</v>
       </c>
       <c r="G46" s="14" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3210,7 +3258,7 @@
         <v>13</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="F47" s="6">
         <v>3</v>
@@ -3227,7 +3275,7 @@
         <v>6</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F48" s="6">
         <v>3</v>
@@ -3244,7 +3292,7 @@
         <v>79</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="F49" s="6">
         <v>3</v>
@@ -3258,7 +3306,7 @@
         <v>13</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="F50" s="6">
         <v>3</v>
@@ -3269,7 +3317,7 @@
     </row>
     <row r="51" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="10" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B51" s="6" t="s">
         <v>44</v>
@@ -3278,7 +3326,7 @@
         <v>41</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E51" s="9" t="s">
         <v>14</v>
@@ -3295,7 +3343,7 @@
         <v>79</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E52" s="9" t="s">
         <v>14</v>
@@ -3312,7 +3360,7 @@
         <v>79</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F53" s="6">
         <v>3</v>
@@ -3326,7 +3374,7 @@
         <v>13</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F54" s="6">
         <v>3</v>
@@ -3354,16 +3402,16 @@
     </row>
     <row r="56" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="10" t="s">
+        <v>458</v>
+      </c>
+      <c r="B56" s="6" t="s">
         <v>459</v>
-      </c>
-      <c r="B56" s="6" t="s">
-        <v>460</v>
       </c>
       <c r="C56" s="7" t="s">
         <v>41</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3374,7 +3422,7 @@
         <v>41</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F57" s="6">
         <v>3</v>
@@ -3411,7 +3459,7 @@
         <v>13</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="F59" s="6">
         <v>4</v>
@@ -3468,10 +3516,10 @@
         <v>13</v>
       </c>
       <c r="D62" s="8" t="s">
+        <v>388</v>
+      </c>
+      <c r="E62" s="9" t="s">
         <v>389</v>
-      </c>
-      <c r="E62" s="9" t="s">
-        <v>390</v>
       </c>
       <c r="F62" s="6">
         <v>3</v>
@@ -3479,7 +3527,7 @@
     </row>
     <row r="63" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="10" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C63" s="7" t="s">
         <v>27</v>
@@ -3488,7 +3536,7 @@
         <v>43</v>
       </c>
       <c r="G63" s="16" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3499,24 +3547,24 @@
         <v>13</v>
       </c>
       <c r="D64" s="8" t="s">
+        <v>377</v>
+      </c>
+      <c r="F64" s="6">
+        <v>3</v>
+      </c>
+      <c r="G64" s="14" t="s">
         <v>378</v>
-      </c>
-      <c r="F64" s="6">
-        <v>3</v>
-      </c>
-      <c r="G64" s="14" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="10" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C65" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D65" s="8" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="E65" s="9" t="s">
         <v>46</v>
@@ -3524,10 +3572,10 @@
     </row>
     <row r="66" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="10" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C66" s="7" t="s">
         <v>27</v>
@@ -3536,7 +3584,7 @@
         <v>43</v>
       </c>
       <c r="G66" s="14" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3550,7 +3598,7 @@
         <v>13</v>
       </c>
       <c r="D67" s="8" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="F67" s="6">
         <v>3</v>
@@ -3564,13 +3612,13 @@
         <v>13</v>
       </c>
       <c r="D68" s="8" t="s">
+        <v>380</v>
+      </c>
+      <c r="F68" s="6">
+        <v>3</v>
+      </c>
+      <c r="G68" s="14" t="s">
         <v>381</v>
-      </c>
-      <c r="F68" s="6">
-        <v>3</v>
-      </c>
-      <c r="G68" s="14" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3581,7 +3629,7 @@
         <v>94</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F69" s="6">
         <v>3</v>
@@ -3598,7 +3646,7 @@
         <v>79</v>
       </c>
       <c r="D70" s="8" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E70" s="9" t="s">
         <v>92</v>
@@ -3621,7 +3669,7 @@
         <v>6</v>
       </c>
       <c r="D71" s="8" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="F71" s="6">
         <v>3</v>
@@ -3638,13 +3686,16 @@
         <v>94</v>
       </c>
       <c r="D72" s="8" t="s">
-        <v>368</v>
+        <v>509</v>
       </c>
       <c r="E72" s="9" t="s">
         <v>115</v>
       </c>
       <c r="F72" s="6">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="G72" s="14" t="s">
+        <v>511</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3678,13 +3729,13 @@
         <v>94</v>
       </c>
       <c r="D74" s="8" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="F74" s="6">
         <v>4</v>
       </c>
       <c r="G74" s="14" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3698,7 +3749,7 @@
         <v>41</v>
       </c>
       <c r="D75" s="8" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="E75" s="9" t="s">
         <v>92</v>
@@ -3741,13 +3792,13 @@
         <v>94</v>
       </c>
       <c r="D77" s="8" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F77" s="6">
         <v>4</v>
       </c>
       <c r="G77" s="14" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="78" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3792,13 +3843,13 @@
         <v>288</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C80" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D80" s="8" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="F80" s="6">
         <v>2</v>
@@ -3903,7 +3954,7 @@
         <v>79</v>
       </c>
       <c r="D86" s="8" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E86" s="13" t="s">
         <v>318</v>
@@ -4061,7 +4112,7 @@
         <v>13</v>
       </c>
       <c r="D96" s="8" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="E96" s="9" t="s">
         <v>270</v>
@@ -4084,7 +4135,7 @@
         <v>79</v>
       </c>
       <c r="D97" s="8" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="E97" s="9" t="s">
         <v>8</v>
@@ -4107,7 +4158,7 @@
         <v>79</v>
       </c>
       <c r="D98" s="8" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="E98" s="9" t="s">
         <v>106</v>
@@ -4130,7 +4181,7 @@
         <v>79</v>
       </c>
       <c r="D99" s="8" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="F99" s="6">
         <v>3</v>
@@ -4141,10 +4192,10 @@
     </row>
     <row r="100" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" s="10" t="s">
+        <v>445</v>
+      </c>
+      <c r="B100" s="6" t="s">
         <v>446</v>
-      </c>
-      <c r="B100" s="6" t="s">
-        <v>447</v>
       </c>
       <c r="C100" s="7" t="s">
         <v>27</v>
@@ -4155,16 +4206,16 @@
     </row>
     <row r="101" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" s="10" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C101" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D101" s="8" t="s">
+        <v>419</v>
+      </c>
+      <c r="G101" s="14" t="s">
         <v>420</v>
-      </c>
-      <c r="G101" s="14" t="s">
-        <v>421</v>
       </c>
     </row>
     <row r="102" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -4178,7 +4229,7 @@
         <v>41</v>
       </c>
       <c r="D102" s="8" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="E102" s="9" t="s">
         <v>266</v>
@@ -4200,13 +4251,13 @@
     </row>
     <row r="104" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" s="10" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C104" s="7" t="s">
         <v>41</v>
       </c>
       <c r="D104" s="8" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="105" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -4220,7 +4271,7 @@
         <v>13</v>
       </c>
       <c r="D105" s="8" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="F105" s="6">
         <v>3</v>
@@ -4228,7 +4279,7 @@
     </row>
     <row r="106" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" s="10" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B106" s="6" t="s">
         <v>144</v>
@@ -4237,7 +4288,7 @@
         <v>41</v>
       </c>
       <c r="D106" s="8" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E106" s="9" t="s">
         <v>26</v>
@@ -4257,18 +4308,18 @@
         <v>13</v>
       </c>
       <c r="D107" s="8" t="s">
+        <v>405</v>
+      </c>
+      <c r="F107" s="6">
+        <v>3</v>
+      </c>
+      <c r="G107" s="14" t="s">
         <v>406</v>
-      </c>
-      <c r="F107" s="6">
-        <v>3</v>
-      </c>
-      <c r="G107" s="14" t="s">
-        <v>407</v>
       </c>
     </row>
     <row r="108" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" s="10" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B108" s="6" t="s">
         <v>159</v>
@@ -4277,15 +4328,15 @@
         <v>6</v>
       </c>
       <c r="D108" s="8" t="s">
+        <v>430</v>
+      </c>
+      <c r="G108" s="14" t="s">
         <v>431</v>
-      </c>
-      <c r="G108" s="14" t="s">
-        <v>432</v>
       </c>
     </row>
     <row r="109" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" s="10" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B109" s="6" t="s">
         <v>104</v>
@@ -4294,7 +4345,7 @@
         <v>13</v>
       </c>
       <c r="D109" s="8" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E109" s="9" t="s">
         <v>46</v>
@@ -4302,7 +4353,7 @@
     </row>
     <row r="110" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" s="10" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B110" s="6" t="s">
         <v>104</v>
@@ -4311,13 +4362,13 @@
         <v>13</v>
       </c>
       <c r="D110" s="8" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E110" s="9" t="s">
         <v>46</v>
       </c>
       <c r="G110" s="16" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="111" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -4331,7 +4382,7 @@
         <v>94</v>
       </c>
       <c r="D111" s="8" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E111" s="12" t="s">
         <v>237</v>
@@ -4340,7 +4391,7 @@
         <v>3</v>
       </c>
       <c r="G111" s="14" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="112" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -4371,7 +4422,7 @@
         <v>79</v>
       </c>
       <c r="D113" s="8" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E113" s="9" t="s">
         <v>21</v>
@@ -4391,7 +4442,7 @@
         <v>79</v>
       </c>
       <c r="D114" s="8" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="F114" s="6">
         <v>3</v>
@@ -4408,13 +4459,13 @@
         <v>41</v>
       </c>
       <c r="D115" s="8" t="s">
+        <v>391</v>
+      </c>
+      <c r="F115" s="6">
+        <v>3</v>
+      </c>
+      <c r="G115" s="14" t="s">
         <v>392</v>
-      </c>
-      <c r="F115" s="6">
-        <v>3</v>
-      </c>
-      <c r="G115" s="14" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="116" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -4479,13 +4530,13 @@
         <v>94</v>
       </c>
       <c r="D119" s="8" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F119" s="6">
         <v>3</v>
       </c>
       <c r="G119" s="14" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="120" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -4499,7 +4550,7 @@
         <v>94</v>
       </c>
       <c r="D120" s="8" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="E120" s="9" t="s">
         <v>92</v>
@@ -4519,7 +4570,7 @@
         <v>79</v>
       </c>
       <c r="D121" s="8" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="E121" s="9" t="s">
         <v>96</v>
@@ -4528,7 +4579,7 @@
         <v>2</v>
       </c>
       <c r="G121" s="14" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="122" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -4542,7 +4593,7 @@
         <v>13</v>
       </c>
       <c r="D122" s="8" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="F122" s="6">
         <v>3</v>
@@ -4562,7 +4613,7 @@
         <v>79</v>
       </c>
       <c r="D123" s="8" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E123" s="9" t="s">
         <v>302</v>
@@ -4571,7 +4622,7 @@
         <v>4</v>
       </c>
       <c r="G123" s="14" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="124" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -4588,7 +4639,7 @@
         <v>63</v>
       </c>
       <c r="E124" s="12" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="F124" s="6">
         <v>4</v>
@@ -4605,7 +4656,7 @@
         <v>79</v>
       </c>
       <c r="D125" s="8" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="F125" s="6">
         <v>3</v>
@@ -4625,7 +4676,7 @@
         <v>94</v>
       </c>
       <c r="D126" s="8" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="E126" s="9" t="s">
         <v>107</v>
@@ -4634,21 +4685,21 @@
         <v>5</v>
       </c>
       <c r="G126" s="14" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="127" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A127" s="4" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B127" s="6" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C127" s="7" t="s">
         <v>41</v>
       </c>
       <c r="D127" s="8" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="128" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -4682,7 +4733,7 @@
         <v>13</v>
       </c>
       <c r="D129" s="8" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="F129" s="6">
         <v>3</v>
@@ -4699,7 +4750,7 @@
         <v>13</v>
       </c>
       <c r="D130" s="8" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E130" s="9" t="s">
         <v>124</v>
@@ -4759,7 +4810,7 @@
         <v>6</v>
       </c>
       <c r="D133" s="8" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="E133" s="9" t="s">
         <v>92</v>
@@ -4839,7 +4890,7 @@
         <v>79</v>
       </c>
       <c r="D137" s="8" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E137" s="9" t="s">
         <v>14</v>
@@ -4848,7 +4899,7 @@
         <v>3</v>
       </c>
       <c r="G137" s="14" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="138" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -4893,7 +4944,7 @@
         <v>41</v>
       </c>
       <c r="D140" s="8" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E140" s="9" t="s">
         <v>124</v>
@@ -4913,7 +4964,7 @@
         <v>41</v>
       </c>
       <c r="D141" s="8" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="E141" s="10" t="s">
         <v>181</v>
@@ -4933,13 +4984,13 @@
         <v>13</v>
       </c>
       <c r="D142" s="8" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F142" s="6">
         <v>3</v>
       </c>
       <c r="G142" s="14" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="143" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -4953,7 +5004,7 @@
         <v>41</v>
       </c>
       <c r="D143" s="8" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="F143" s="6">
         <v>3</v>
@@ -4970,7 +5021,7 @@
         <v>79</v>
       </c>
       <c r="D144" s="8" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E144" s="9" t="s">
         <v>127</v>
@@ -4984,13 +5035,13 @@
         <v>114</v>
       </c>
       <c r="B145" s="6" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="C145" s="7" t="s">
         <v>94</v>
       </c>
       <c r="D145" s="8" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="E145" s="9" t="s">
         <v>115</v>
@@ -5001,7 +5052,7 @@
     </row>
     <row r="146" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A146" s="4" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B146" s="6" t="s">
         <v>24</v>
@@ -5010,7 +5061,7 @@
         <v>41</v>
       </c>
       <c r="D146" s="8" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="147" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -5024,7 +5075,7 @@
         <v>13</v>
       </c>
       <c r="D147" s="8" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E147" s="9" t="s">
         <v>14</v>
@@ -5055,13 +5106,13 @@
         <v>13</v>
       </c>
       <c r="D149" s="8" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="F149" s="6">
         <v>3</v>
       </c>
       <c r="G149" s="14" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="150" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -5095,7 +5146,7 @@
         <v>41</v>
       </c>
       <c r="D151" s="8" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="F151" s="6">
         <v>3</v>
@@ -5106,13 +5157,13 @@
         <v>287</v>
       </c>
       <c r="B152" s="6" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C152" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D152" s="8" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="F152" s="6">
         <v>2</v>
@@ -5120,16 +5171,16 @@
     </row>
     <row r="153" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A153" s="10" t="s">
+        <v>464</v>
+      </c>
+      <c r="B153" s="6" t="s">
         <v>465</v>
-      </c>
-      <c r="B153" s="6" t="s">
-        <v>466</v>
       </c>
       <c r="C153" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D153" s="8" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E153" s="9" t="s">
         <v>14</v>
@@ -5154,7 +5205,7 @@
     </row>
     <row r="155" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A155" s="10" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B155" s="6" t="s">
         <v>126</v>
@@ -5163,7 +5214,7 @@
         <v>13</v>
       </c>
       <c r="D155" s="8" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E155" s="9" t="s">
         <v>14</v>
@@ -5172,7 +5223,7 @@
         <v>1</v>
       </c>
       <c r="G155" s="15" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="156" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -5186,7 +5237,7 @@
         <v>94</v>
       </c>
       <c r="D156" s="8" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E156" s="9" t="s">
         <v>14</v>
@@ -5200,22 +5251,22 @@
     </row>
     <row r="157" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A157" s="10" t="s">
+        <v>432</v>
+      </c>
+      <c r="B157" s="6" t="s">
         <v>433</v>
-      </c>
-      <c r="B157" s="6" t="s">
-        <v>434</v>
       </c>
       <c r="C157" s="7" t="s">
         <v>79</v>
       </c>
       <c r="D157" s="8" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="E157" s="9" t="s">
+        <v>434</v>
+      </c>
+      <c r="G157" s="16" t="s">
         <v>435</v>
-      </c>
-      <c r="G157" s="16" t="s">
-        <v>436</v>
       </c>
     </row>
     <row r="158" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -5229,7 +5280,7 @@
         <v>41</v>
       </c>
       <c r="D158" s="8" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="E158" s="9" t="s">
         <v>179</v>
@@ -5243,10 +5294,10 @@
     </row>
     <row r="159" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A159" s="10" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B159" s="6" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C159" s="7" t="s">
         <v>94</v>
@@ -5255,15 +5306,15 @@
         <v>34</v>
       </c>
       <c r="E159" s="9" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="160" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A160" s="10" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B160" s="6" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C160" s="7" t="s">
         <v>94</v>
@@ -5272,7 +5323,7 @@
         <v>34</v>
       </c>
       <c r="G160" s="14" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="161" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -5303,7 +5354,7 @@
         <v>79</v>
       </c>
       <c r="D162" s="8" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="E162" s="9" t="s">
         <v>246</v>
@@ -5312,7 +5363,7 @@
         <v>2</v>
       </c>
       <c r="G162" s="14" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="163" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -5326,13 +5377,13 @@
         <v>41</v>
       </c>
       <c r="D163" s="8" t="s">
+        <v>393</v>
+      </c>
+      <c r="F163" s="6">
+        <v>3</v>
+      </c>
+      <c r="G163" s="14" t="s">
         <v>394</v>
-      </c>
-      <c r="F163" s="6">
-        <v>3</v>
-      </c>
-      <c r="G163" s="14" t="s">
-        <v>395</v>
       </c>
     </row>
     <row r="164" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -5346,13 +5397,13 @@
         <v>13</v>
       </c>
       <c r="D164" s="8" t="s">
+        <v>402</v>
+      </c>
+      <c r="F164" s="6">
+        <v>3</v>
+      </c>
+      <c r="G164" s="14" t="s">
         <v>403</v>
-      </c>
-      <c r="F164" s="6">
-        <v>3</v>
-      </c>
-      <c r="G164" s="14" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="165" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -5366,13 +5417,16 @@
         <v>94</v>
       </c>
       <c r="D165" s="8" t="s">
-        <v>368</v>
+        <v>519</v>
       </c>
       <c r="E165" s="9" t="s">
         <v>118</v>
       </c>
       <c r="F165" s="6">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="G165" s="14" t="s">
+        <v>521</v>
       </c>
     </row>
     <row r="166" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -5386,7 +5440,7 @@
         <v>13</v>
       </c>
       <c r="D166" s="8" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="E166" s="9" t="s">
         <v>21</v>
@@ -5403,7 +5457,7 @@
         <v>13</v>
       </c>
       <c r="D167" s="8" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E167" s="9" t="s">
         <v>46</v>
@@ -5412,7 +5466,7 @@
         <v>4</v>
       </c>
       <c r="G167" s="14" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="168" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -5426,7 +5480,7 @@
         <v>13</v>
       </c>
       <c r="D168" s="8" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E168" s="9" t="s">
         <v>92</v>
@@ -5480,7 +5534,7 @@
         <v>94</v>
       </c>
       <c r="D171" s="8" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="E171" s="9" t="s">
         <v>124</v>
@@ -5500,7 +5554,7 @@
         <v>13</v>
       </c>
       <c r="D172" s="8" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F172" s="6">
         <v>3</v>
@@ -5511,13 +5565,13 @@
         <v>289</v>
       </c>
       <c r="B173" s="6" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="C173" s="7" t="s">
         <v>41</v>
       </c>
       <c r="D173" s="8" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="E173" s="9" t="s">
         <v>14</v>
@@ -5534,7 +5588,7 @@
         <v>13</v>
       </c>
       <c r="D174" s="8" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="F174" s="6">
         <v>3</v>
@@ -5551,7 +5605,7 @@
         <v>94</v>
       </c>
       <c r="D175" s="8" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="F175" s="6">
         <v>3</v>
@@ -5562,7 +5616,7 @@
     </row>
     <row r="176" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A176" s="10" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B176" s="6" t="s">
         <v>183</v>
@@ -5571,46 +5625,46 @@
         <v>27</v>
       </c>
       <c r="D176" s="8" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="177" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A177" s="10" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B177" s="6" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="C177" s="7" t="s">
         <v>41</v>
       </c>
       <c r="D177" s="8" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="E177" s="9" t="s">
         <v>14</v>
       </c>
       <c r="G177" s="14" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="178" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A178" s="10" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C178" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D178" s="8" t="s">
+        <v>474</v>
+      </c>
+      <c r="G178" s="15" t="s">
         <v>475</v>
-      </c>
-      <c r="G178" s="15" t="s">
-        <v>476</v>
       </c>
     </row>
     <row r="179" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A179" s="10" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B179" s="6" t="s">
         <v>316</v>
@@ -5619,18 +5673,18 @@
         <v>6</v>
       </c>
       <c r="D179" s="8" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="E179" s="9" t="s">
         <v>14</v>
       </c>
       <c r="G179" s="15" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="180" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A180" s="10" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B180" s="6" t="s">
         <v>48</v>
@@ -5639,7 +5693,7 @@
         <v>41</v>
       </c>
       <c r="D180" s="8" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="E180" s="9" t="s">
         <v>14</v>
@@ -5647,7 +5701,7 @@
     </row>
     <row r="181" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A181" s="10" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B181" s="6" t="s">
         <v>48</v>
@@ -5656,27 +5710,27 @@
         <v>13</v>
       </c>
       <c r="D181" s="8" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="E181" s="9" t="s">
         <v>14</v>
       </c>
       <c r="G181" s="14" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="182" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A182" s="10" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B182" s="6" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="C182" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D182" s="8" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="E182" s="9" t="s">
         <v>14</v>
@@ -5684,21 +5738,21 @@
     </row>
     <row r="183" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A183" s="10" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B183" s="6" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C183" s="7" t="s">
         <v>27</v>
       </c>
       <c r="D183" s="8" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="184" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A184" s="10" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B184" s="6" t="s">
         <v>48</v>
@@ -5707,7 +5761,7 @@
         <v>6</v>
       </c>
       <c r="D184" s="8" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="E184" s="9" t="s">
         <v>14</v>
@@ -5718,13 +5772,13 @@
         <v>47</v>
       </c>
       <c r="B185" s="6" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="C185" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D185" s="8" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="E185" s="9" t="s">
         <v>14</v>
@@ -5732,7 +5786,7 @@
     </row>
     <row r="186" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A186" s="10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B186" s="6" t="s">
         <v>48</v>
@@ -5741,18 +5795,18 @@
         <v>13</v>
       </c>
       <c r="D186" s="8" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="E186" s="9" t="s">
         <v>14</v>
       </c>
       <c r="G186" s="15" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="187" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A187" s="10" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B187" s="6" t="s">
         <v>183</v>
@@ -5761,21 +5815,21 @@
         <v>27</v>
       </c>
       <c r="D187" s="8" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="188" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A188" s="10" t="s">
+        <v>498</v>
+      </c>
+      <c r="B188" s="6" t="s">
         <v>499</v>
-      </c>
-      <c r="B188" s="6" t="s">
-        <v>500</v>
       </c>
       <c r="C188" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D188" s="8" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="E188" s="9" t="s">
         <v>14</v>
@@ -5783,27 +5837,27 @@
     </row>
     <row r="189" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A189" s="10" t="s">
+        <v>500</v>
+      </c>
+      <c r="B189" s="6" t="s">
         <v>501</v>
-      </c>
-      <c r="B189" s="6" t="s">
-        <v>502</v>
       </c>
       <c r="C189" s="7" t="s">
         <v>41</v>
       </c>
       <c r="D189" s="8" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="E189" s="9" t="s">
         <v>14</v>
       </c>
       <c r="G189" s="15" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="190" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A190" s="10" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B190" s="6" t="s">
         <v>120</v>
@@ -5812,33 +5866,121 @@
         <v>6</v>
       </c>
       <c r="D190" s="8" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="E190" s="9" t="s">
         <v>14</v>
       </c>
       <c r="G190" s="15" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="191" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A191" s="10" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B191" s="6" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="C191" s="7" t="s">
         <v>41</v>
       </c>
       <c r="D191" s="8" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="E191" s="9" t="s">
         <v>14</v>
       </c>
       <c r="G191" s="14" t="s">
-        <v>507</v>
+        <v>506</v>
+      </c>
+    </row>
+    <row r="192" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
+      <c r="A192" s="10" t="s">
+        <v>508</v>
+      </c>
+      <c r="B192" s="6" t="s">
+        <v>510</v>
+      </c>
+      <c r="C192" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D192" s="8" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="193" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
+      <c r="A193" s="10" t="s">
+        <v>512</v>
+      </c>
+      <c r="B193" s="6" t="s">
+        <v>514</v>
+      </c>
+      <c r="C193" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D193" s="8" t="s">
+        <v>509</v>
+      </c>
+      <c r="E193" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G193" s="14" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="194" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
+      <c r="A194" s="10" t="s">
+        <v>515</v>
+      </c>
+      <c r="B194" s="6" t="s">
+        <v>517</v>
+      </c>
+      <c r="C194" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="D194" s="8" t="s">
+        <v>509</v>
+      </c>
+      <c r="E194" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="195" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
+      <c r="A195" s="10" t="s">
+        <v>516</v>
+      </c>
+      <c r="B195" s="6" t="s">
+        <v>517</v>
+      </c>
+      <c r="C195" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="D195" s="8" t="s">
+        <v>509</v>
+      </c>
+      <c r="E195" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G195" s="15" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="196" spans="1:7" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
+      <c r="A196" s="10" t="s">
+        <v>520</v>
+      </c>
+      <c r="B196" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="C196" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D196" s="8" t="s">
+        <v>519</v>
+      </c>
+      <c r="E196" s="9" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -6143,10 +6285,19 @@
     <hyperlink ref="A191" r:id="rId297" display="https://leetcode.cn/problems/reverse-words-in-a-string/" xr:uid="{4B2C101B-F768-4107-A3A8-689A2F608E3D}"/>
     <hyperlink ref="E191" r:id="rId298" xr:uid="{A73A0A4E-FB11-41B3-80E5-2FA40B81A50D}"/>
     <hyperlink ref="E173" r:id="rId299" xr:uid="{8D50CBDB-2242-4BBB-B694-184E0070104C}"/>
+    <hyperlink ref="A192" r:id="rId300" display="https://leetcode.cn/problems/minimum-operations-to-exceed-threshold-value-ii/" xr:uid="{1E11646A-D940-446C-8E1B-6F3CD471DAEC}"/>
+    <hyperlink ref="A193" r:id="rId301" xr:uid="{EECF5DCB-F6DA-4CC6-B808-B6D1A0FD2EA7}"/>
+    <hyperlink ref="E193" r:id="rId302" location="%E6%80%9D%E8%B7%AF" xr:uid="{7DC750A1-BD6D-404C-A7A2-3CC13D80ECC3}"/>
+    <hyperlink ref="A194" r:id="rId303" display="https://leetcode.cn/problems/find-the-index-of-the-first-occurrence-in-a-string/" xr:uid="{023E2A06-6F13-495C-B896-F7241E8F25EB}"/>
+    <hyperlink ref="A195" r:id="rId304" display="https://leetcode.cn/problems/repeated-substring-pattern/" xr:uid="{1EBC7A26-002F-442F-A7E1-A7CB3DFA8EAF}"/>
+    <hyperlink ref="E194" r:id="rId305" location="%E7%AE%97%E6%B3%95%E5%85%AC%E5%BC%80%E8%AF%BE" xr:uid="{B0445983-C761-4027-9892-5CFEFE2DE00C}"/>
+    <hyperlink ref="E195" r:id="rId306" xr:uid="{8F8CDCBB-6C08-48EE-8A19-679B6978F012}"/>
+    <hyperlink ref="A196" r:id="rId307" display="https://leetcode.cn/problems/shortest-subarray-with-or-at-least-k-i/" xr:uid="{207B1343-AACF-47A4-AB70-78314E7B029D}"/>
+    <hyperlink ref="E196" r:id="rId308" xr:uid="{86B685E1-568D-4D4B-B0DF-6A49B35DCE2D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId300"/>
+    <tablePart r:id="rId309"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>